<commit_message>
PSP sheet upload 10/1
</commit_message>
<xml_diff>
--- a/PSP_Sheets/PSP_Sheet_박진영.xlsx
+++ b/PSP_Sheets/PSP_Sheet_박진영.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjy20\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjy20\OneDrive - 서강대학교\2019년 2학기\융합소프트웨어종합설계\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B898908-9E42-4817-96E6-07768D6DC25F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372ACFC9-A824-4D3E-957C-2E99EE1B2DF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -259,10 +259,6 @@
   </si>
   <si>
     <t>팀명: 2조</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디어 선정 및 프로젝트 계획서 작성</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -290,6 +286,195 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>아이디어 선정 및 프로젝트 계획서 작성 / GitHub Storage 생성 및 초대</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 계획서 수정 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Competetion, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>주요기능)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 계획서 바탕으로 프레젠테이션 준비</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>프레젠테이션 발표 준비</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>새로운</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> Target Application 관련 경쟁 서비스 조사 및 차별점 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ideation</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use Case Diagram </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>바탕으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 프레젠테이션 자료 작성</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Target Application </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 계획서 최종 수정 </t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Node js 강의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 수강</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>프로토타입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 제작 - 기본 Form UI</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로그인, 데이터</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 입력, 입력 결과를 보여주는 프로토타입 제작</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +484,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -368,6 +553,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +612,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -456,6 +659,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -843,7 +1049,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -852,7 +1058,7 @@
     <col min="2" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="11.453125" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="46.453125" customWidth="1"/>
+    <col min="6" max="6" width="62.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -876,7 +1082,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3"/>
     </row>
@@ -918,88 +1124,208 @@
         <v>100</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="14">
+        <v>43717</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>60</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="14">
+        <v>43717</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>30</v>
+      </c>
+      <c r="E8" s="16">
+        <v>150</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="4"/>
+      <c r="A9" s="14">
+        <v>43718</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>60</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="14">
+        <v>43726</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>60</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="15">
+        <v>43729</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <v>120</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="14">
+        <v>43734</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="17">
+        <v>60</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="14">
+        <v>43734</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17">
+        <v>60</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>43736</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>120</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="4"/>
+      <c r="A15" s="14">
+        <v>43737</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17">
+        <v>120</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="14">
+        <v>43738</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D16" s="9">
+        <v>90</v>
+      </c>
+      <c r="E16" s="17">
+        <v>340</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>

</xml_diff>